<commit_message>
added body Temperature and heart rate
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bodyWeight.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bodyWeight.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$68</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="502">
   <si>
     <t>Path</t>
   </si>
@@ -956,6 +956,140 @@
   </si>
   <si>
     <t>363714003 |Interprets|</t>
+  </si>
+  <si>
+    <t>valueQuantity</t>
+  </si>
+  <si>
+    <t>Observation.value[x].id</t>
+  </si>
+  <si>
+    <t>Observation.value[x].extension</t>
+  </si>
+  <si>
+    <t>Observation.value[x].value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal
+</t>
+  </si>
+  <si>
+    <t>Numerical value (with implicit precision)</t>
+  </si>
+  <si>
+    <t>The value of the measured amount. The value includes an implicit precision in the presentation of the value.</t>
+  </si>
+  <si>
+    <t>The implicit precision in the value should always be honored. Monetary values have their own rules for handling precision (refer to standard accounting text books).</t>
+  </si>
+  <si>
+    <t>Precision is handled implicitly in almost all cases of measurement.</t>
+  </si>
+  <si>
+    <t>Quantity.value</t>
+  </si>
+  <si>
+    <t>SN.2  / CQ - N/A</t>
+  </si>
+  <si>
+    <t>PQ.value, CO.value, MO.value, IVL.high or IVL.low depending on the value</t>
+  </si>
+  <si>
+    <t>Observation.value[x].comparator</t>
+  </si>
+  <si>
+    <t>&lt; | &lt;= | &gt;= | &gt; - how to understand the value</t>
+  </si>
+  <si>
+    <t>How the value should be understood and represented - whether the actual value is greater or less than the stated value due to measurement issues; e.g. if the comparator is "&lt;" , then the real value is &lt; stated value.</t>
+  </si>
+  <si>
+    <t>Need a framework for handling measures where the value is &lt;5ug/L or &gt;400mg/L due to the limitations of measuring methodology.</t>
+  </si>
+  <si>
+    <t>If there is no comparator, then there is no modification of the value</t>
+  </si>
+  <si>
+    <t>How the Quantity should be understood and represented.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/quantity-comparator|4.0.1</t>
+  </si>
+  <si>
+    <t>Quantity.comparator</t>
+  </si>
+  <si>
+    <t>SN.1  / CQ.1</t>
+  </si>
+  <si>
+    <t>IVL properties</t>
+  </si>
+  <si>
+    <t>Observation.value[x].unit</t>
+  </si>
+  <si>
+    <t>Unit representation</t>
+  </si>
+  <si>
+    <t>A human-readable form of the unit.</t>
+  </si>
+  <si>
+    <t>There are many representations for units of measure and in many contexts, particular representations are fixed and required. I.e. mcg for micrograms.</t>
+  </si>
+  <si>
+    <t>https://johnmoehrke.github.io/MHV-PGHD/ValueSet/mhv-body-weights</t>
+  </si>
+  <si>
+    <t>Quantity.unit</t>
+  </si>
+  <si>
+    <t>(see OBX.6 etc.) / CQ.2</t>
+  </si>
+  <si>
+    <t>PQ.unit</t>
+  </si>
+  <si>
+    <t>Observation.value[x].system</t>
+  </si>
+  <si>
+    <t>System that defines coded unit form</t>
+  </si>
+  <si>
+    <t>The identification of the system that provides the coded form of the unit.</t>
+  </si>
+  <si>
+    <t>Need to know the system that defines the coded form of the unit.</t>
+  </si>
+  <si>
+    <t>Quantity.system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qty-3
+</t>
+  </si>
+  <si>
+    <t>CO.codeSystem, PQ.translation.codeSystem</t>
+  </si>
+  <si>
+    <t>Observation.value[x].code</t>
+  </si>
+  <si>
+    <t>Coded form of the unit</t>
+  </si>
+  <si>
+    <t>A computer processable form of the unit in some unit representation system.</t>
+  </si>
+  <si>
+    <t>The preferred system is UCUM, but SNOMED CT can also be used (for customary units) or ISO 4217 for currency.  The context of use may additionally require a code from a particular system.</t>
+  </si>
+  <si>
+    <t>Need a computable form of the unit that is fixed across all forms. UCUM provides this for quantities, but SNOMED CT provides many units of interest.</t>
+  </si>
+  <si>
+    <t>Quantity.code</t>
+  </si>
+  <si>
+    <t>PQ.code, MO.currency, PQ.translation.code</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1612,7 +1746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO60"/>
+  <dimension ref="A1:AO68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1645,7 +1779,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="66.0703125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -5379,16 +5513,14 @@
         <v>45</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AB32" s="2"/>
       <c r="AC32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AE32" t="s" s="2">
         <v>286</v>
@@ -5426,9 +5558,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="B33" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
         <v>45</v>
       </c>
@@ -5437,7 +5571,7 @@
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5446,22 +5580,22 @@
         <v>45</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>204</v>
+        <v>287</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5486,13 +5620,13 @@
         <v>45</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>303</v>
+        <v>45</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>45</v>
@@ -5510,7 +5644,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5519,7 +5653,7 @@
         <v>55</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>67</v>
@@ -5528,35 +5662,35 @@
         <v>45</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>155</v>
+        <v>294</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>45</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>307</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>45</v>
@@ -5568,20 +5702,16 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>308</v>
+        <v>69</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>311</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
       </c>
@@ -5605,13 +5735,13 @@
         <v>45</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>312</v>
+        <v>45</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>313</v>
+        <v>45</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>45</v>
@@ -5629,53 +5759,53 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>306</v>
+        <v>71</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>314</v>
+        <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>316</v>
+        <v>72</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>317</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>45</v>
@@ -5687,20 +5817,18 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>319</v>
+        <v>75</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>320</v>
+        <v>76</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>321</v>
+        <v>77</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>323</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5736,19 +5864,19 @@
         <v>45</v>
       </c>
       <c r="AA35" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="AC35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD35" t="s" s="2">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>318</v>
+        <v>82</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5760,7 +5888,7 @@
         <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>45</v>
@@ -5769,10 +5897,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>324</v>
+        <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>325</v>
+        <v>72</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5783,7 +5911,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5794,7 +5922,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
@@ -5803,21 +5931,23 @@
         <v>45</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>204</v>
+        <v>301</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="N36" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>305</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5841,13 +5971,13 @@
         <v>45</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>330</v>
+        <v>45</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>331</v>
+        <v>45</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
@@ -5865,7 +5995,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5883,24 +6013,24 @@
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>332</v>
+        <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>335</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5911,36 +6041,36 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>339</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>340</v>
+        <v>312</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="P37" s="2"/>
+      <c r="P37" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="Q37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5960,13 +6090,13 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5984,7 +6114,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6005,10 +6135,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -6019,7 +6149,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6030,7 +6160,7 @@
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>45</v>
@@ -6039,21 +6169,21 @@
         <v>45</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>346</v>
+        <v>57</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -6077,13 +6207,11 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="X38" s="2"/>
       <c r="Y38" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -6101,7 +6229,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6119,24 +6247,24 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>353</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6147,7 +6275,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6156,21 +6284,21 @@
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>355</v>
+        <v>97</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>356</v>
+        <v>328</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N39" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6218,7 +6346,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6227,7 +6355,7 @@
         <v>55</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>45</v>
+        <v>332</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>67</v>
@@ -6236,24 +6364,24 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>361</v>
+        <v>333</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>362</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6264,7 +6392,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6273,22 +6401,22 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>364</v>
+        <v>132</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>365</v>
+        <v>335</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>366</v>
+        <v>336</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>368</v>
+        <v>338</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6337,19 +6465,19 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>369</v>
+        <v>67</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6358,10 +6486,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>370</v>
+        <v>325</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>371</v>
+        <v>340</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6372,7 +6500,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>372</v>
+        <v>341</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6383,7 +6511,7 @@
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6395,16 +6523,20 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>69</v>
+        <v>342</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>345</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6428,13 +6560,13 @@
         <v>45</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>45</v>
+        <v>346</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>45</v>
+        <v>347</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>45</v>
@@ -6452,7 +6584,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>71</v>
+        <v>341</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6461,10 +6593,10 @@
         <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>45</v>
+        <v>348</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>45</v>
@@ -6473,10 +6605,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>72</v>
+        <v>349</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6487,18 +6619,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>74</v>
+        <v>351</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>45</v>
@@ -6510,18 +6642,20 @@
         <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>75</v>
+        <v>204</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>76</v>
+        <v>352</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>77</v>
+        <v>353</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N42" s="2"/>
+        <v>354</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>355</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
       </c>
@@ -6545,13 +6679,13 @@
         <v>45</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>45</v>
+        <v>356</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>45</v>
+        <v>357</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>45</v>
@@ -6569,7 +6703,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>82</v>
+        <v>350</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6581,65 +6715,65 @@
         <v>45</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>45</v>
+        <v>358</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>72</v>
+        <v>360</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>375</v>
+        <v>45</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>75</v>
+        <v>363</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>78</v>
+        <v>366</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6688,7 +6822,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6700,7 +6834,7 @@
         <v>45</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>45</v>
@@ -6709,10 +6843,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>155</v>
+        <v>369</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6723,7 +6857,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6734,7 +6868,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6746,15 +6880,17 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>381</v>
+        <v>204</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="M44" s="2"/>
+        <v>372</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6779,13 +6915,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6803,7 +6939,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6812,7 +6948,7 @@
         <v>55</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>384</v>
+        <v>45</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>67</v>
@@ -6821,24 +6957,24 @@
         <v>45</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>45</v>
+        <v>376</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>45</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6849,7 +6985,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6861,16 +6997,20 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="K45" t="s" s="2">
-        <v>388</v>
-      </c>
       <c r="L45" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>384</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6894,13 +7034,13 @@
         <v>45</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>45</v>
+        <v>385</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>45</v>
+        <v>386</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>45</v>
@@ -6918,7 +7058,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6927,7 +7067,7 @@
         <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>384</v>
+        <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>67</v>
@@ -6939,10 +7079,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6953,7 +7093,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6964,7 +7104,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6976,20 +7116,18 @@
         <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>204</v>
+        <v>390</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>393</v>
       </c>
-      <c r="M46" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>395</v>
-      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -7013,13 +7151,13 @@
         <v>45</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>397</v>
+        <v>45</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>45</v>
@@ -7037,7 +7175,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7055,24 +7193,24 @@
         <v>45</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>316</v>
+        <v>396</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>45</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7083,7 +7221,7 @@
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
@@ -7095,20 +7233,18 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>204</v>
+        <v>399</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>402</v>
       </c>
-      <c r="M47" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>404</v>
-      </c>
+      <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7132,13 +7268,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>405</v>
+        <v>45</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>406</v>
+        <v>45</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -7156,13 +7292,13 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
@@ -7174,19 +7310,19 @@
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>316</v>
+        <v>405</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>45</v>
+        <v>406</v>
       </c>
     </row>
     <row r="48" hidden="true">
@@ -7202,7 +7338,7 @@
         <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
@@ -7222,9 +7358,11 @@
       <c r="L48" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="M48" s="2"/>
+      <c r="M48" t="s" s="2">
+        <v>411</v>
+      </c>
       <c r="N48" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7279,13 +7417,13 @@
         <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>413</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
@@ -7294,10 +7432,10 @@
         <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>45</v>
+        <v>414</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7308,7 +7446,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7334,10 +7472,10 @@
         <v>57</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>414</v>
+        <v>69</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>415</v>
+        <v>70</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7388,7 +7526,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>413</v>
+        <v>71</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7400,7 +7538,7 @@
         <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>45</v>
@@ -7409,10 +7547,10 @@
         <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>385</v>
+        <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>416</v>
+        <v>72</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7427,14 +7565,14 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
@@ -7443,19 +7581,19 @@
         <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>418</v>
+        <v>75</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>419</v>
+        <v>76</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>420</v>
+        <v>77</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>421</v>
+        <v>78</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7505,7 +7643,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>417</v>
+        <v>82</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7517,7 +7655,7 @@
         <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
@@ -7526,10 +7664,10 @@
         <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>422</v>
+        <v>45</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>423</v>
+        <v>72</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
@@ -7540,41 +7678,43 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>45</v>
+        <v>419</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I51" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>425</v>
+        <v>75</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>422</v>
+      </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
       </c>
@@ -7622,7 +7762,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7634,7 +7774,7 @@
         <v>45</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>45</v>
@@ -7643,10 +7783,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>422</v>
+        <v>45</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>429</v>
+        <v>155</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7657,7 +7797,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7668,7 +7808,7 @@
         <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>45</v>
@@ -7677,23 +7817,19 @@
         <v>45</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>364</v>
+        <v>425</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>434</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>45</v>
       </c>
@@ -7741,16 +7877,16 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>45</v>
+        <v>428</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>67</v>
@@ -7762,10 +7898,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7776,7 +7912,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7799,13 +7935,13 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>57</v>
+        <v>425</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>69</v>
+        <v>432</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>70</v>
+        <v>433</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7856,7 +7992,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>71</v>
+        <v>431</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7865,10 +8001,10 @@
         <v>55</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>45</v>
+        <v>428</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>45</v>
@@ -7877,10 +8013,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>45</v>
+        <v>429</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>72</v>
+        <v>434</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -7891,18 +8027,18 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>45</v>
@@ -7914,18 +8050,20 @@
         <v>45</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>75</v>
+        <v>204</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>76</v>
+        <v>436</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>77</v>
+        <v>437</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N54" s="2"/>
+        <v>438</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>439</v>
+      </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
       </c>
@@ -7949,13 +8087,13 @@
         <v>45</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>45</v>
+        <v>440</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>45</v>
+        <v>441</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>45</v>
@@ -7973,31 +8111,31 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>82</v>
+        <v>435</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>45</v>
+        <v>442</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>45</v>
+        <v>443</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>72</v>
+        <v>360</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8008,11 +8146,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>375</v>
+        <v>45</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -8025,25 +8163,25 @@
         <v>45</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>75</v>
+        <v>204</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>376</v>
+        <v>445</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>377</v>
+        <v>446</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>78</v>
+        <v>447</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>378</v>
+        <v>448</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
@@ -8068,13 +8206,13 @@
         <v>45</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>45</v>
+        <v>449</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>45</v>
+        <v>450</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>45</v>
@@ -8092,7 +8230,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>379</v>
+        <v>444</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8104,19 +8242,19 @@
         <v>45</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>45</v>
+        <v>442</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>45</v>
+        <v>443</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>155</v>
+        <v>360</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8127,7 +8265,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8135,7 +8273,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F56" t="s" s="2">
         <v>55</v>
@@ -8147,22 +8285,20 @@
         <v>45</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>204</v>
+        <v>452</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>443</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>219</v>
+        <v>455</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8187,13 +8323,13 @@
         <v>45</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>221</v>
+        <v>45</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>222</v>
+        <v>45</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>45</v>
@@ -8211,10 +8347,10 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>55</v>
@@ -8229,16 +8365,16 @@
         <v>45</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>444</v>
+        <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>226</v>
+        <v>456</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>227</v>
+        <v>45</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>45</v>
@@ -8246,7 +8382,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8266,23 +8402,19 @@
         <v>45</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>446</v>
+        <v>57</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>459</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>45</v>
       </c>
@@ -8330,7 +8462,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8348,24 +8480,24 @@
         <v>45</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>449</v>
+        <v>45</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>294</v>
+        <v>429</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>295</v>
+        <v>460</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>296</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8376,7 +8508,7 @@
         <v>43</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>45</v>
@@ -8385,23 +8517,21 @@
         <v>45</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>204</v>
+        <v>462</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>453</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>465</v>
+      </c>
+      <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>45</v>
       </c>
@@ -8425,13 +8555,13 @@
         <v>45</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>303</v>
+        <v>45</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
@@ -8449,16 +8579,16 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>304</v>
+        <v>45</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>67</v>
@@ -8470,10 +8600,10 @@
         <v>45</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>155</v>
+        <v>466</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>305</v>
+        <v>467</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>45</v>
@@ -8484,18 +8614,18 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>307</v>
+        <v>45</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>45</v>
@@ -8504,23 +8634,21 @@
         <v>45</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>204</v>
+        <v>469</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>308</v>
+        <v>470</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>309</v>
+        <v>471</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>311</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>45</v>
       </c>
@@ -8544,13 +8672,13 @@
         <v>45</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>312</v>
+        <v>45</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>313</v>
+        <v>45</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>45</v>
@@ -8568,7 +8696,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8586,24 +8714,24 @@
         <v>45</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>314</v>
+        <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>315</v>
+        <v>466</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>316</v>
+        <v>473</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>317</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>455</v>
+        <v>474</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8614,7 +8742,7 @@
         <v>43</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>45</v>
@@ -8623,22 +8751,22 @@
         <v>45</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>45</v>
+        <v>408</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>456</v>
+        <v>475</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>457</v>
+        <v>476</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>367</v>
+        <v>477</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>368</v>
+        <v>478</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -8687,7 +8815,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>455</v>
+        <v>474</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8708,20 +8836,966 @@
         <v>45</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>370</v>
+        <v>479</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>371</v>
+        <v>480</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO60" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM61" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AN61" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO61" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM62" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AN62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO62" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" hidden="true">
+      <c r="A63" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F63" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H63" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="I63" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J63" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K63" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="L63" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="O63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE63" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="AF63" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG63" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI63" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM63" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AN63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO63" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" hidden="true">
+      <c r="A64" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="F64" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I64" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J64" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K64" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="O64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P64" s="2"/>
+      <c r="Q64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W64" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="X64" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="Z64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE64" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="AF64" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AG64" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI64" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AM64" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AN64" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AO64" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" hidden="true">
+      <c r="A65" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="O65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AM65" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AN65" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO65" t="s" s="2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="66" hidden="true">
+      <c r="A66" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F66" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM66" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AN66" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO66" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" hidden="true">
+      <c r="A67" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K67" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="N67" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="O67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="AM67" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AN67" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO67" t="s" s="2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="68" hidden="true">
+      <c r="A68" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F68" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="O68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="AM68" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="AN68" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO68" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO60">
+  <autoFilter ref="A1:AO68">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8731,7 +9805,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI59">
+  <conditionalFormatting sqref="A2:AI67">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>